<commit_message>
-added tool status excel sheet
</commit_message>
<xml_diff>
--- a/230523 Tools Status.xlsx
+++ b/230523 Tools Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Minecraft\Minecraft Java\Lootdebugs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3161432E-F58F-4D65-BB7D-D2FE12AAC773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4641FC1-DF8D-4E18-A2A6-DD22ED2A1FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6870" windowWidth="29040" windowHeight="15840" xr2:uid="{B0D27BBE-F0C9-4E7A-A617-7E5DE5D11701}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{B0D27BBE-F0C9-4E7A-A617-7E5DE5D11701}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>Mixer Barrel</t>
   </si>
   <si>
-    <t>not implemented</t>
-  </si>
-  <si>
     <t>Shield</t>
   </si>
   <si>
@@ -126,6 +123,10 @@
   </si>
   <si>
     <t>Turret Ammo</t>
+  </si>
+  <si>
+    <t>model missing;
+rotation missing;</t>
   </si>
 </sst>
 </file>
@@ -574,7 +575,7 @@
   <dimension ref="A4:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,16 +628,16 @@
         <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -654,16 +655,16 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -677,13 +678,13 @@
         <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>13</v>
@@ -692,7 +693,7 @@
         <v>13</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -703,16 +704,16 @@
         <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>18</v>
+      <c r="E8" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>15</v>

</xml_diff>